<commit_message>
v0.1.6 - Updated Pagado/Pendiente report (Feb 20 cut-off)
</commit_message>
<xml_diff>
--- a/administrador/resumen_general.xlsx
+++ b/administrador/resumen_general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/administrador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253E7983-B9AE-504E-A820-B0681EFDA95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF6BC5-D6E4-FB4E-B70F-447290AABD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{0B03E385-4D70-1443-97FA-03D8B48AE23F}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16360" xr2:uid="{0B03E385-4D70-1443-97FA-03D8B48AE23F}"/>
   </bookViews>
   <sheets>
     <sheet name="pagado_pendiente" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,202 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="141">
+  <dxfs count="146">
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="hair">
@@ -993,6 +1188,198 @@
         <extend val="0"/>
         <color indexed="10"/>
       </font>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="hair">
           <color indexed="64"/>
@@ -1409,22 +1796,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1501,6 +1872,13 @@
     </dxf>
     <dxf>
       <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <left style="hair">
           <color indexed="64"/>
         </left>
@@ -1523,7 +1901,7 @@
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="hair">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -1533,7 +1911,14 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -1549,7 +1934,14 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -1565,13 +1957,13 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="hair">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -1581,6 +1973,13 @@
     </dxf>
     <dxf>
       <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <left style="hair">
           <color indexed="64"/>
         </left>
@@ -1603,7 +2002,7 @@
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="hair">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -1613,6 +2012,13 @@
     </dxf>
     <dxf>
       <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <left style="hair">
           <color indexed="64"/>
         </left>
@@ -1629,7 +2035,14 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -1645,7 +2058,14 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -1661,13 +2081,13 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="hair">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -1677,6 +2097,13 @@
     </dxf>
     <dxf>
       <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <left style="hair">
           <color indexed="64"/>
         </left>
@@ -1692,11 +2119,13 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="hair">
           <color indexed="64"/>
@@ -1720,748 +2149,13 @@
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="hair">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Bookshelf Symbol 7"/>
-        <family val="2"/>
-        <charset val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Bookshelf Symbol 7"/>
-        <family val="2"/>
-        <charset val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Bookshelf Symbol 7"/>
-        <family val="2"/>
-        <charset val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Bookshelf Symbol 7"/>
-        <family val="2"/>
-        <charset val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="#,##0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2775,6 +2469,210 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Bookshelf Symbol 7"/>
+        <family val="2"/>
+        <charset val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Bookshelf Symbol 7"/>
+        <family val="2"/>
+        <charset val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Bookshelf Symbol 7"/>
+        <family val="2"/>
+        <charset val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Bookshelf Symbol 7"/>
+        <family val="2"/>
+        <charset val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="#,##0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="#,##0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="#,##0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="#,##0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2858,6 +2756,118 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3096,57 +3106,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:F47" totalsRowShown="0" headerRowDxfId="140" dataDxfId="138" headerRowBorderDxfId="139" tableBorderDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:F47" totalsRowShown="0" headerRowDxfId="145" dataDxfId="143" headerRowBorderDxfId="144" tableBorderDxfId="142">
   <autoFilter ref="A2:F47" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="136"/>
-    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas_Pagado" dataDxfId="134"/>
-    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Recibo_Inicial_Pagado" dataDxfId="133"/>
-    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Pólizas_Pendiente" dataDxfId="132"/>
-    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Recibo_Inicial_Pendiente" dataDxfId="131"/>
+    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="141"/>
+    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="140"/>
+    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas_Pagado" dataDxfId="139"/>
+    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Recibo_Inicial_Pagado" dataDxfId="138"/>
+    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Pólizas_Pendiente" dataDxfId="137"/>
+    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Recibo_Inicial_Pendiente" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
   <autoFilter ref="N2:Y6" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="108"/>
-    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="107" dataCellStyle="Porcentaje"/>
-    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="106" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="105" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="104" dataCellStyle="Porcentaje"/>
-    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="103" dataCellStyle="Porcentaje"/>
-    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="102" dataCellStyle="Porcentaje"/>
-    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="101" dataCellStyle="Porcentaje"/>
-    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="100" dataCellStyle="Porcentaje"/>
-    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="99"/>
-    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="131" dataCellStyle="Porcentaje"/>
+    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="130" dataCellStyle="Porcentaje"/>
+    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="129" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="128" dataCellStyle="Porcentaje"/>
+    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="127" dataCellStyle="Porcentaje"/>
+    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="126" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="125" dataCellStyle="Porcentaje"/>
+    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="124" dataCellStyle="Porcentaje"/>
+    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="123"/>
+    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
   <autoFilter ref="A2:L49" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="96"/>
-    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="95"/>
-    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="94"/>
-    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="93"/>
-    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="92"/>
-    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="91"/>
-    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="90"/>
-    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="89"/>
-    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="110"/>
+    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3171,26 +3181,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A2:J60" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="122"/>
-    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="117" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="114"/>
-    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="113" dataCellStyle="Porcentaje"/>
+    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="105"/>
+    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="100" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="98"/>
+    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="97"/>
+    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="96" dataCellStyle="Porcentaje"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="112" headerRowBorderDxfId="111" tableBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93">
   <autoFilter ref="M2:AB4" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{092EDBAB-8D8A-EA4D-9E0C-E48510EA1510}" name="Polizas_Pagadas_Año_Anterior"/>
@@ -3536,8 +3546,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3556,7 +3566,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="36">
-        <v>46070</v>
+        <v>46073</v>
       </c>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
@@ -3607,7 +3617,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2">
         <v>2043</v>
@@ -3616,28 +3626,28 @@
         <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>3018.58</v>
+        <v>61004.82</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>72844.100000000006</v>
       </c>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>3273.67</v>
+        <v>3018.58</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -3649,22 +3659,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4">
-        <v>36437.94</v>
+        <v>3273.67</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>72844.100000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3681,10 +3691,10 @@
         <v>7184.56</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4">
-        <v>1935.08</v>
+        <v>15064.07</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3701,10 +3711,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>672629.43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3721,10 +3731,10 @@
         <v>1584.48</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>2435.65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3849,16 +3859,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>-6.95</v>
+        <v>0</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -3889,16 +3899,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2">
-        <v>2856</v>
+        <v>2692</v>
       </c>
       <c r="C18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4">
-        <v>1809.19</v>
+        <v>0</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -3909,16 +3919,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>0</v>
+        <v>-6.95</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -3929,16 +3939,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="4">
-        <v>0</v>
+        <v>1809.19</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -3949,10 +3959,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -3969,10 +3979,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -3989,10 +3999,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -4001,18 +4011,18 @@
         <v>0</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4">
-        <v>0</v>
+        <v>36777.25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -4029,7 +4039,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2">
         <v>2043</v>
@@ -4049,10 +4059,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -4069,30 +4079,30 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B27" s="2">
         <v>2856</v>
       </c>
       <c r="C27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>2561.44</v>
+        <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>5165.8599999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -4109,10 +4119,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B29" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -4121,35 +4131,35 @@
         <v>0</v>
       </c>
       <c r="E29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>24131.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="4">
-        <v>0</v>
+        <v>2561.44</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4">
-        <v>0</v>
+        <v>5165.8599999999997</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2">
         <v>2043</v>
@@ -4161,15 +4171,15 @@
         <v>0</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="4">
-        <v>0</v>
+        <v>24131.27</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2">
         <v>2043</v>
@@ -4189,7 +4199,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2">
         <v>2043</v>
@@ -4209,10 +4219,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -4229,7 +4239,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B35" s="2">
         <v>2043</v>
@@ -4241,15 +4251,15 @@
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="4">
-        <v>0</v>
+        <v>5102.97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B36" s="2">
         <v>2043</v>
@@ -4269,10 +4279,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2">
-        <v>2692</v>
+        <v>2856</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -4289,7 +4299,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2">
         <v>2043</v>
@@ -4309,10 +4319,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B39" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -4329,10 +4339,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B40" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -4349,7 +4359,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B41" s="2">
         <v>2043</v>
@@ -4369,10 +4379,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B42" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
@@ -4389,10 +4399,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B43" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -4477,101 +4487,101 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="89" priority="46" stopIfTrue="1">
+      <formula>$Q47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="47" stopIfTrue="1">
+      <formula>$Q46=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="expression" dxfId="84" priority="49" stopIfTrue="1">
+      <formula>$Q96=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="50" stopIfTrue="1">
+      <formula>$Q95=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:D47 F47">
+    <cfRule type="expression" dxfId="82" priority="67" stopIfTrue="1">
+      <formula>$Q47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="68" stopIfTrue="1">
+      <formula>$Q46=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" dxfId="74" priority="65" stopIfTrue="1">
+      <formula>$Q47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="66" stopIfTrue="1">
+      <formula>$Q46=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A46">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="87" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A46">
-    <cfRule type="expression" dxfId="86" priority="13" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="14" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="84" priority="31" stopIfTrue="1">
-      <formula>$Q47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="32" stopIfTrue="1">
-      <formula>$Q46=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="82" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B46">
-    <cfRule type="expression" dxfId="81" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="79" priority="34" stopIfTrue="1">
-      <formula>$Q96=1</formula>
+  <conditionalFormatting sqref="C4:D46">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+      <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="35" stopIfTrue="1">
-      <formula>$Q95=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47:D47 F47">
-    <cfRule type="expression" dxfId="77" priority="52" stopIfTrue="1">
-      <formula>$Q47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="53" stopIfTrue="1">
-      <formula>$Q46=1</formula>
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D3">
-    <cfRule type="expression" dxfId="75" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D46">
-    <cfRule type="expression" dxfId="74" priority="7" stopIfTrue="1">
+  <conditionalFormatting sqref="E4:E46">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F46">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="72" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E46">
-    <cfRule type="expression" dxfId="71" priority="1" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="2" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="69" priority="50" stopIfTrue="1">
-      <formula>$Q47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="51" stopIfTrue="1">
-      <formula>$Q46=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="67" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
       <formula>$S$34=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F46">
-    <cfRule type="expression" dxfId="66" priority="3" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="4" stopIfTrue="1">
-      <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6486,150 +6496,146 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:A49">
+    <cfRule type="expression" dxfId="69" priority="18" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="19" stopIfTrue="1">
+      <formula>+#REF!="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B49">
+    <cfRule type="expression" dxfId="67" priority="16" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="17" stopIfTrue="1">
+      <formula>+#REF!="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C49">
+    <cfRule type="expression" dxfId="65" priority="12" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:H49">
+    <cfRule type="expression" dxfId="64" priority="13" stopIfTrue="1">
+      <formula>+#REF!="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D49">
+    <cfRule type="expression" dxfId="63" priority="11" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E49">
+    <cfRule type="expression" dxfId="62" priority="10" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F49">
+    <cfRule type="expression" dxfId="61" priority="9" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G49">
+    <cfRule type="expression" dxfId="60" priority="8" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H49">
+    <cfRule type="expression" dxfId="59" priority="7" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I49">
+    <cfRule type="expression" dxfId="58" priority="5" stopIfTrue="1">
+      <formula>$R3="i"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="14" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J49">
+    <cfRule type="expression" dxfId="56" priority="2" stopIfTrue="1">
+      <formula>$S3="i"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="6" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K49">
+    <cfRule type="expression" dxfId="54" priority="3" stopIfTrue="1">
+      <formula>$T3="i"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="15" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L49">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
+      <formula>$U3="i"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="4" stopIfTrue="1">
+      <formula>$B3&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N3:N6">
-    <cfRule type="expression" dxfId="54" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="31" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O6">
-    <cfRule type="expression" dxfId="53" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="30" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P6">
-    <cfRule type="expression" dxfId="52" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="29" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q6">
-    <cfRule type="expression" dxfId="51" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="28" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R6">
-    <cfRule type="expression" dxfId="50" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="27" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S6">
-    <cfRule type="expression" dxfId="49" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="26" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T6">
-    <cfRule type="expression" dxfId="48" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="25" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U6">
-    <cfRule type="expression" dxfId="47" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V6">
-    <cfRule type="expression" dxfId="46" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="23" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W6">
-    <cfRule type="expression" dxfId="45" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X6">
-    <cfRule type="expression" dxfId="44" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="21" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y6">
-    <cfRule type="expression" dxfId="43" priority="20" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A49">
-    <cfRule type="expression" dxfId="42" priority="19" stopIfTrue="1">
-      <formula>+#REF!="p"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A49">
-    <cfRule type="expression" dxfId="41" priority="18" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B49">
-    <cfRule type="expression" dxfId="40" priority="17" stopIfTrue="1">
-      <formula>+#REF!="p"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B49">
-    <cfRule type="expression" dxfId="39" priority="16" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:H49">
-    <cfRule type="expression" dxfId="38" priority="13" stopIfTrue="1">
-      <formula>+#REF!="p"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C49">
-    <cfRule type="expression" dxfId="37" priority="12" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D49">
-    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E49">
-    <cfRule type="expression" dxfId="35" priority="10" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F49">
-    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G49">
-    <cfRule type="expression" dxfId="33" priority="8" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H49">
-    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I49">
-    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
-      <formula>$R3="i"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="14" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J49">
-    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
-      <formula>$S3="i"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="6" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K49">
-    <cfRule type="expression" dxfId="27" priority="3" stopIfTrue="1">
-      <formula>$T3="i"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="15" stopIfTrue="1">
-      <formula>$B3&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L49">
-    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
-      <formula>$U3="i"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6648,7 +6654,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -10138,98 +10144,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A60">
-    <cfRule type="expression" dxfId="23" priority="23">
+    <cfRule type="expression" dxfId="38" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="23">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="expression" dxfId="21" priority="21">
+    <cfRule type="expression" dxfId="36" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="21">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C60">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="15">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D60">
-    <cfRule type="expression" dxfId="17" priority="14">
+    <cfRule type="expression" dxfId="32" priority="19" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="14">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E60">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="30" priority="13">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F60">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F60">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="26" priority="12">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G60">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="24" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H60">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I60">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="20" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J60">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J60">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
v0.1.7 - Renamed RI columns to Total Pagado/Pendiente
- Replaced all RI Pagado references with Total Pagado
- Replaced all RI Pendiente references with Total Pendiente
- Updated KPI cards, table headers, and chart titles
- Updated Excel data with new column names
</commit_message>
<xml_diff>
--- a/administrador/resumen_general.xlsx
+++ b/administrador/resumen_general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/administrador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF6BC5-D6E4-FB4E-B70F-447290AABD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E778549-509C-AD4C-A0F5-1FB8C005CC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16360" xr2:uid="{0B03E385-4D70-1443-97FA-03D8B48AE23F}"/>
   </bookViews>
@@ -404,16 +404,16 @@
     <t>%_Asesores_con_pol_Pagada_GMM</t>
   </si>
   <si>
-    <t>Recibo_Inicial_Pagado</t>
-  </si>
-  <si>
     <t>Pólizas_Pagado</t>
   </si>
   <si>
     <t>Pólizas_Pendiente</t>
   </si>
   <si>
-    <t>Recibo_Inicial_Pendiente</t>
+    <t>Total_Pagado</t>
+  </si>
+  <si>
+    <t>Total_Pendiente</t>
   </si>
 </sst>
 </file>
@@ -755,7 +755,85 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="146">
+  <dxfs count="152">
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="hair">
@@ -3106,57 +3184,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:F47" totalsRowShown="0" headerRowDxfId="145" dataDxfId="143" headerRowBorderDxfId="144" tableBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:F47" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150" tableBorderDxfId="148">
   <autoFilter ref="A2:F47" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="141"/>
-    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="140"/>
-    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas_Pagado" dataDxfId="139"/>
-    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Recibo_Inicial_Pagado" dataDxfId="138"/>
-    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Pólizas_Pendiente" dataDxfId="137"/>
-    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Recibo_Inicial_Pendiente" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="146"/>
+    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas_Pagado" dataDxfId="145"/>
+    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Total_Pagado" dataDxfId="144"/>
+    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Pólizas_Pendiente" dataDxfId="143"/>
+    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Total_Pendiente" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140">
   <autoFilter ref="N2:Y6" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="132"/>
-    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="131" dataCellStyle="Porcentaje"/>
-    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="130" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="129" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="128" dataCellStyle="Porcentaje"/>
-    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="127" dataCellStyle="Porcentaje"/>
-    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="126" dataCellStyle="Porcentaje"/>
-    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="125" dataCellStyle="Porcentaje"/>
-    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="124" dataCellStyle="Porcentaje"/>
-    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="123"/>
-    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="137" dataCellStyle="Porcentaje"/>
+    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="136" dataCellStyle="Porcentaje"/>
+    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="135" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="134" dataCellStyle="Porcentaje"/>
+    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="133" dataCellStyle="Porcentaje"/>
+    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="132" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="131" dataCellStyle="Porcentaje"/>
+    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="130" dataCellStyle="Porcentaje"/>
+    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="129"/>
+    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="A2:L49" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="114"/>
-    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="110"/>
-    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="109"/>
-    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="122"/>
+    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="119"/>
+    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="118"/>
+    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="117"/>
+    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="116"/>
+    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="115"/>
+    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3181,26 +3259,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="A2:J60" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="105"/>
-    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="100" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="99"/>
-    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="98"/>
-    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="97"/>
-    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="96" dataCellStyle="Porcentaje"/>
+    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="110"/>
+    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="107"/>
+    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="106" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="105"/>
+    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="104"/>
+    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="103"/>
+    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="102" dataCellStyle="Porcentaje"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="101" headerRowBorderDxfId="100" tableBorderDxfId="99">
   <autoFilter ref="M2:AB4" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{092EDBAB-8D8A-EA4D-9E0C-E48510EA1510}" name="Polizas_Pagadas_Año_Anterior"/>
@@ -3547,7 +3625,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3581,13 +3659,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>124</v>
@@ -3605,13 +3683,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>104105.63</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>225651.58</v>
       </c>
       <c r="I3" s="7"/>
     </row>
@@ -3626,13 +3704,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>61004.82</v>
+        <v>74359.210000000006</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>72844.100000000006</v>
+        <v>108385.48</v>
       </c>
       <c r="I4" s="8"/>
     </row>
@@ -3647,13 +3725,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>3018.58</v>
+        <v>71251.41</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>37782.11</v>
       </c>
       <c r="I5" s="8"/>
     </row>
@@ -3668,13 +3746,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="4">
-        <v>3273.67</v>
+        <v>52982.99</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>21966.880000000001</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3688,13 +3766,13 @@
         <v>2</v>
       </c>
       <c r="D7" s="4">
-        <v>7184.56</v>
+        <v>40909.81</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>
       </c>
       <c r="F7" s="4">
-        <v>15064.07</v>
+        <v>204839.8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3708,13 +3786,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>27079.33</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>801637.94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3728,13 +3806,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="4">
-        <v>1584.48</v>
+        <v>26005.4</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>2435.65</v>
+        <v>99845.58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3748,13 +3826,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>22054.400000000001</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>75875.25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3768,13 +3846,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>20077.400000000001</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>42810.25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3788,13 +3866,13 @@
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>0</v>
+        <v>14887.38</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>14887.38</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3808,13 +3886,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>0</v>
+        <v>11945.29</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
+        <v>66315.25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3828,13 +3906,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="4">
-        <v>0</v>
+        <v>11532.26</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
       </c>
       <c r="F14" s="4">
-        <v>21932.89</v>
+        <v>58958.98</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3848,13 +3926,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>0</v>
+        <v>9688.8700000000008</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>0</v>
+        <v>24855.21</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3868,13 +3946,13 @@
         <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>0</v>
+        <v>9281.48</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>34668.69</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3888,13 +3966,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="4">
-        <v>0</v>
+        <v>8821.32</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
+        <v>11272.92</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3908,13 +3986,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="4">
-        <v>0</v>
+        <v>7991.52</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
       </c>
       <c r="F18" s="4">
-        <v>0</v>
+        <v>55306.96</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3928,13 +4006,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>-6.95</v>
+        <v>7460.84</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
+        <v>15352.07</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3948,13 +4026,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="4">
-        <v>1809.19</v>
+        <v>6716.14</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
+        <v>43873.2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3968,13 +4046,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="4">
-        <v>0</v>
+        <v>6639.64</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <v>0</v>
+        <v>8336.92</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3988,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>0</v>
+        <v>6196.74</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -4008,13 +4086,13 @@
         <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>0</v>
+        <v>5895.02</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
       <c r="F23" s="4">
-        <v>36777.25</v>
+        <v>88859</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -4028,13 +4106,13 @@
         <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
+        <v>5745.69</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>0</v>
+        <v>22496</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -4048,13 +4126,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>0</v>
+        <v>5138.51</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>0</v>
+        <v>10277.030000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -4068,13 +4146,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
+        <v>4663.49</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <v>0</v>
+        <v>3167.47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -4088,13 +4166,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>0</v>
+        <v>4487.59</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>38209.879999999997</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4108,13 +4186,13 @@
         <v>0</v>
       </c>
       <c r="D28" s="4">
-        <v>0</v>
+        <v>4192.72</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="4">
-        <v>0</v>
+        <v>23946.42</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4128,13 +4206,13 @@
         <v>0</v>
       </c>
       <c r="D29" s="4">
-        <v>0</v>
+        <v>4095.39</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
+        <v>63114.42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4148,13 +4226,13 @@
         <v>1</v>
       </c>
       <c r="D30" s="4">
-        <v>2561.44</v>
+        <v>3993.98</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
       </c>
       <c r="F30" s="4">
-        <v>5165.8599999999997</v>
+        <v>26539.81</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4168,13 +4246,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>0</v>
+        <v>3904.72</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="4">
-        <v>24131.27</v>
+        <v>49420.01</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -4188,7 +4266,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="4">
-        <v>0</v>
+        <v>3151.08</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -4208,13 +4286,13 @@
         <v>0</v>
       </c>
       <c r="D33" s="4">
-        <v>0</v>
+        <v>2852.69</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
       </c>
       <c r="F33" s="4">
-        <v>0</v>
+        <v>1575.88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -4228,13 +4306,13 @@
         <v>0</v>
       </c>
       <c r="D34" s="4">
-        <v>0</v>
+        <v>2833.03</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
+        <v>4506.84</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -4248,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>0</v>
+        <v>2133.91</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
@@ -4268,13 +4346,13 @@
         <v>0</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>1721.93</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>0</v>
+        <v>22676.73</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -4288,7 +4366,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="4">
-        <v>0</v>
+        <v>1712.03</v>
       </c>
       <c r="E37" s="3">
         <v>0</v>
@@ -4308,13 +4386,13 @@
         <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>0</v>
+        <v>1345.8</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>0</v>
+        <v>4779.2299999999996</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -4328,13 +4406,13 @@
         <v>0</v>
       </c>
       <c r="D39" s="4">
-        <v>0</v>
+        <v>1297.97</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
+        <v>32930.35</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -4348,13 +4426,13 @@
         <v>0</v>
       </c>
       <c r="D40" s="4">
-        <v>0</v>
+        <v>1269.82</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="4">
-        <v>0</v>
+        <v>49303.64</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -4368,13 +4446,13 @@
         <v>0</v>
       </c>
       <c r="D41" s="4">
-        <v>0</v>
+        <v>651.19000000000005</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
+        <v>46859.360000000001</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -4394,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="4">
-        <v>0</v>
+        <v>18020.830000000002</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -4414,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>0</v>
+        <v>127958.49</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -4434,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="4">
-        <v>0</v>
+        <v>10092.959999999999</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -4454,7 +4532,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>0</v>
+        <v>15118.28</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -4474,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0</v>
+        <v>12739.06</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -4488,38 +4566,64 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="89" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="52" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="53" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="84" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="55" stopIfTrue="1">
       <formula>$Q96=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="56" stopIfTrue="1">
       <formula>$Q95=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:D47 F47">
-    <cfRule type="expression" dxfId="82" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="73" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="74" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="71" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="72" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A46">
+    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+      <formula>$S$34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>$S$34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B46">
+    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C46">
     <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
@@ -4527,60 +4631,47 @@
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
+  <conditionalFormatting sqref="C3">
     <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>$S$34=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B46">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="E4:E46">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D46">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:D3">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
-      <formula>$S$34=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E46">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F46">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D46">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>$S$34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F46">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6497,145 +6588,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A49">
-    <cfRule type="expression" dxfId="69" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="19" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B49">
-    <cfRule type="expression" dxfId="67" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="16" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="17" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C49">
-    <cfRule type="expression" dxfId="65" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="12" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:H49">
-    <cfRule type="expression" dxfId="64" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="13" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D49">
-    <cfRule type="expression" dxfId="63" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E49">
-    <cfRule type="expression" dxfId="62" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="10" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F49">
-    <cfRule type="expression" dxfId="61" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G49">
-    <cfRule type="expression" dxfId="60" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H49">
-    <cfRule type="expression" dxfId="59" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I49">
-    <cfRule type="expression" dxfId="58" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="5" stopIfTrue="1">
       <formula>$R3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="14" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J49">
-    <cfRule type="expression" dxfId="56" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="2" stopIfTrue="1">
       <formula>$S3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K49">
-    <cfRule type="expression" dxfId="54" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="3" stopIfTrue="1">
       <formula>$T3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="15" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L49">
-    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="1" stopIfTrue="1">
       <formula>$U3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="4" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N6">
-    <cfRule type="expression" dxfId="50" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="31" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O6">
-    <cfRule type="expression" dxfId="49" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="30" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P6">
-    <cfRule type="expression" dxfId="48" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="29" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q6">
-    <cfRule type="expression" dxfId="47" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="28" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R6">
-    <cfRule type="expression" dxfId="46" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="27" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S6">
-    <cfRule type="expression" dxfId="45" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="26" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T6">
-    <cfRule type="expression" dxfId="44" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="25" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U6">
-    <cfRule type="expression" dxfId="43" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V6">
-    <cfRule type="expression" dxfId="42" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="23" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W6">
-    <cfRule type="expression" dxfId="41" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X6">
-    <cfRule type="expression" dxfId="40" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="21" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y6">
-    <cfRule type="expression" dxfId="39" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10144,98 +10235,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A60">
-    <cfRule type="expression" dxfId="38" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="23">
+    <cfRule type="expression" dxfId="43" priority="23">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="expression" dxfId="36" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="21">
+    <cfRule type="expression" dxfId="41" priority="21">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C60">
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="15">
+    <cfRule type="expression" dxfId="39" priority="15">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D60">
-    <cfRule type="expression" dxfId="32" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="19" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="37" priority="14">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E60">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F60">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F60">
-    <cfRule type="expression" dxfId="26" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="17" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G60">
-    <cfRule type="expression" dxfId="24" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H60">
-    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I60">
-    <cfRule type="expression" dxfId="20" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J60">
-    <cfRule type="cellIs" dxfId="18" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J60">
-    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
v0.1.8 - Updated Pagado/Pendiente data (Feb 23 cut-off)
</commit_message>
<xml_diff>
--- a/administrador/resumen_general.xlsx
+++ b/administrador/resumen_general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/administrador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E778549-509C-AD4C-A0F5-1FB8C005CC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8163DCCA-D7B4-584C-8378-98534862C8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16360" xr2:uid="{0B03E385-4D70-1443-97FA-03D8B48AE23F}"/>
   </bookViews>
@@ -797,6 +797,45 @@
     </dxf>
     <dxf>
       <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <left style="hair">
           <color indexed="64"/>
         </left>
@@ -824,84 +863,6 @@
           <color indexed="64"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
           <color indexed="64"/>
         </right>
         <top style="hair">
@@ -1950,6 +1911,22 @@
     </dxf>
     <dxf>
       <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1960,6 +1937,29 @@
         <left style="hair">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="hair">
           <color indexed="64"/>
         </right>
@@ -1973,13 +1973,13 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top style="hair">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -2002,7 +2002,7 @@
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="hair">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -2012,6 +2012,22 @@
     </dxf>
     <dxf>
       <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2019,7 +2035,23 @@
     </dxf>
     <dxf>
       <border>
-        <left style="thin">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -2035,7 +2067,14 @@
     </dxf>
     <dxf>
       <border>
-        <left style="thin">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -2051,6 +2090,22 @@
     </dxf>
     <dxf>
       <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2058,7 +2113,7 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
@@ -2074,13 +2129,27 @@
     </dxf>
     <dxf>
       <border>
-        <left style="hair">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="hair">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top style="hair">
           <color indexed="64"/>
         </top>
         <bottom style="hair">
@@ -2090,6 +2159,38 @@
     </dxf>
     <dxf>
       <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2116,107 +2217,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3625,7 +3625,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3644,7 +3644,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="36">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
@@ -3686,10 +3686,10 @@
         <v>104105.63</v>
       </c>
       <c r="E3" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="4">
-        <v>225651.58</v>
+        <v>285524.36</v>
       </c>
       <c r="I3" s="7"/>
     </row>
@@ -3707,10 +3707,10 @@
         <v>74359.210000000006</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
-        <v>108385.48</v>
+        <v>173883</v>
       </c>
       <c r="I4" s="8"/>
     </row>
@@ -3763,16 +3763,16 @@
         <v>2856</v>
       </c>
       <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>52275.28</v>
+      </c>
+      <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="4">
-        <v>40909.81</v>
-      </c>
-      <c r="E7" s="3">
-        <v>3</v>
-      </c>
       <c r="F7" s="4">
-        <v>204839.8</v>
+        <v>193474.33</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3789,7 +3789,7 @@
         <v>27079.33</v>
       </c>
       <c r="E8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="4">
         <v>801637.94</v>
@@ -3809,10 +3809,10 @@
         <v>26005.4</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
-        <v>99845.58</v>
+        <v>122577.57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3829,10 +3829,10 @@
         <v>22054.400000000001</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>75875.25</v>
+        <v>99901.29</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3877,7 +3877,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2">
         <v>2692</v>
@@ -3886,18 +3886,18 @@
         <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>11945.29</v>
+        <v>14217.61</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>66315.25</v>
+        <v>113740.88</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2">
         <v>2692</v>
@@ -3906,38 +3906,38 @@
         <v>0</v>
       </c>
       <c r="D14" s="4">
-        <v>11532.26</v>
+        <v>11945.29</v>
       </c>
       <c r="E14" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14" s="4">
-        <v>58958.98</v>
+        <v>66315.25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>9688.8700000000008</v>
+        <v>11532.26</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="4">
-        <v>24855.21</v>
+        <v>58958.98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2">
         <v>2043</v>
@@ -3946,18 +3946,18 @@
         <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>9281.48</v>
+        <v>9688.8700000000008</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="4">
-        <v>34668.69</v>
+        <v>24855.21</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>2043</v>
@@ -3966,38 +3966,38 @@
         <v>0</v>
       </c>
       <c r="D17" s="4">
-        <v>8821.32</v>
+        <v>9281.48</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>11272.92</v>
+        <v>34668.69</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18" s="4">
-        <v>7991.52</v>
+        <v>8821.32</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
       </c>
       <c r="F18" s="4">
-        <v>55306.96</v>
+        <v>11272.92</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>2692</v>
@@ -4006,78 +4006,78 @@
         <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>7460.84</v>
+        <v>7991.52</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>15352.07</v>
+        <v>55306.96</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2">
-        <v>2856</v>
+        <v>2692</v>
       </c>
       <c r="C20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>6716.14</v>
+        <v>7460.84</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
       </c>
       <c r="F20" s="4">
-        <v>43873.2</v>
+        <v>15352.07</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2">
         <v>2856</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="4">
-        <v>6639.64</v>
+        <v>6716.14</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <v>8336.92</v>
+        <v>43873.2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>6196.74</v>
+        <v>6639.64</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
+        <v>8336.92</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2">
         <v>2692</v>
@@ -4086,18 +4086,18 @@
         <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>5895.02</v>
+        <v>6463.82</v>
       </c>
       <c r="E23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
-        <v>88859</v>
+        <v>60745.99</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2">
         <v>2043</v>
@@ -4106,18 +4106,18 @@
         <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>5745.69</v>
+        <v>6196.74</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>22496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>2043</v>
@@ -4126,58 +4126,58 @@
         <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>5138.51</v>
+        <v>6125.03</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>10277.030000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B26" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>4663.49</v>
+        <v>5895.02</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>3167.47</v>
+        <v>87131.78</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>4487.59</v>
+        <v>5745.69</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>38209.879999999997</v>
+        <v>22496</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B28" s="2">
         <v>2043</v>
@@ -4186,78 +4186,78 @@
         <v>0</v>
       </c>
       <c r="D28" s="4">
-        <v>4192.72</v>
+        <v>5620.13</v>
       </c>
       <c r="E28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4">
-        <v>23946.42</v>
+        <v>47704.6</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
       </c>
       <c r="D29" s="4">
-        <v>4095.39</v>
+        <v>5138.51</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>63114.42</v>
+        <v>10277.030000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B30" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="4">
-        <v>3993.98</v>
+        <v>4663.49</v>
       </c>
       <c r="E30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="4">
-        <v>26539.81</v>
+        <v>3167.47</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B31" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>3904.72</v>
+        <v>4487.59</v>
       </c>
       <c r="E31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>49420.01</v>
+        <v>38209.879999999997</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B32" s="2">
         <v>2043</v>
@@ -4266,38 +4266,38 @@
         <v>0</v>
       </c>
       <c r="D32" s="4">
-        <v>3151.08</v>
+        <v>4192.72</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
       <c r="F32" s="4">
-        <v>0</v>
+        <v>23946.42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B33" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C33" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4">
-        <v>2852.69</v>
+        <v>3993.98</v>
       </c>
       <c r="E33" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="4">
-        <v>1575.88</v>
+        <v>26539.81</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B34" s="2">
         <v>2043</v>
@@ -4306,18 +4306,18 @@
         <v>0</v>
       </c>
       <c r="D34" s="4">
-        <v>2833.03</v>
+        <v>3151.08</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>4506.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2">
         <v>2043</v>
@@ -4326,18 +4326,18 @@
         <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>2133.91</v>
+        <v>2852.69</v>
       </c>
       <c r="E35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="4">
-        <v>5102.97</v>
+        <v>1575.88</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2">
         <v>2043</v>
@@ -4346,38 +4346,38 @@
         <v>0</v>
       </c>
       <c r="D36" s="4">
-        <v>1721.93</v>
+        <v>2833.03</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>22676.73</v>
+        <v>4506.84</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37" s="4">
-        <v>1712.03</v>
+        <v>2133.91</v>
       </c>
       <c r="E37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
+        <v>5102.97</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2">
         <v>2043</v>
@@ -4386,58 +4386,58 @@
         <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>1345.8</v>
+        <v>1721.93</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>4779.2299999999996</v>
+        <v>22676.73</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B39" s="2">
-        <v>2692</v>
+        <v>2856</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
       </c>
       <c r="D39" s="4">
-        <v>1297.97</v>
+        <v>1712.03</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>32930.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
       </c>
       <c r="D40" s="4">
-        <v>1269.82</v>
+        <v>1297.97</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="4">
-        <v>49303.64</v>
+        <v>32930.35</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B41" s="2">
         <v>2043</v>
@@ -4446,18 +4446,18 @@
         <v>0</v>
       </c>
       <c r="D41" s="4">
-        <v>651.19000000000005</v>
+        <v>1269.82</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>46859.360000000001</v>
+        <v>49303.64</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B42" s="2">
         <v>2043</v>
@@ -4466,21 +4466,21 @@
         <v>0</v>
       </c>
       <c r="D42" s="4">
-        <v>0</v>
+        <v>651.19000000000005</v>
       </c>
       <c r="E42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="4">
-        <v>18020.830000000002</v>
+        <v>61733.46</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -4492,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>127958.49</v>
+        <v>18020.830000000002</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -4566,90 +4566,90 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="95" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="71" stopIfTrue="1">
+      <formula>$Q46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="70" stopIfTrue="1">
       <formula>$Q47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="53" stopIfTrue="1">
-      <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="90" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="74" stopIfTrue="1">
+      <formula>$Q95=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="73" stopIfTrue="1">
       <formula>$Q96=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="56" stopIfTrue="1">
-      <formula>$Q95=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:D47 F47">
-    <cfRule type="expression" dxfId="88" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="92" stopIfTrue="1">
+      <formula>$Q46=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="91" stopIfTrue="1">
       <formula>$Q47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
-      <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="80" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="89" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="90" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A46">
-    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B46">
-    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C46">
-    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>$S$34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D46">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E46">
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
-      <formula>$S$34=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D46">
     <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
@@ -4657,7 +4657,7 @@
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
+  <conditionalFormatting sqref="E3">
     <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
@@ -6588,145 +6588,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A49">
-    <cfRule type="expression" dxfId="75" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="19" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B49">
-    <cfRule type="expression" dxfId="73" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="16" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="17" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C49">
-    <cfRule type="expression" dxfId="71" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="12" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:H49">
-    <cfRule type="expression" dxfId="70" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="13" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D49">
-    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="11" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E49">
-    <cfRule type="expression" dxfId="68" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="10" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F49">
-    <cfRule type="expression" dxfId="67" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G49">
-    <cfRule type="expression" dxfId="66" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H49">
-    <cfRule type="expression" dxfId="65" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I49">
-    <cfRule type="expression" dxfId="64" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="5" stopIfTrue="1">
       <formula>$R3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="14" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J49">
-    <cfRule type="expression" dxfId="62" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="2" stopIfTrue="1">
       <formula>$S3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K49">
-    <cfRule type="expression" dxfId="60" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="3" stopIfTrue="1">
       <formula>$T3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="15" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L49">
-    <cfRule type="expression" dxfId="58" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
       <formula>$U3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N6">
-    <cfRule type="expression" dxfId="56" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="31" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O6">
-    <cfRule type="expression" dxfId="55" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="30" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P6">
-    <cfRule type="expression" dxfId="54" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q6">
-    <cfRule type="expression" dxfId="53" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="28" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R6">
-    <cfRule type="expression" dxfId="52" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="27" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S6">
-    <cfRule type="expression" dxfId="51" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="26" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T6">
-    <cfRule type="expression" dxfId="50" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="25" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U6">
-    <cfRule type="expression" dxfId="49" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V6">
-    <cfRule type="expression" dxfId="48" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="23" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W6">
-    <cfRule type="expression" dxfId="47" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X6">
-    <cfRule type="expression" dxfId="46" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="21" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y6">
-    <cfRule type="expression" dxfId="45" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10235,98 +10235,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A60">
-    <cfRule type="expression" dxfId="44" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="23">
+    <cfRule type="expression" dxfId="40" priority="23">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="expression" dxfId="42" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="21">
+    <cfRule type="expression" dxfId="38" priority="21">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C60">
-    <cfRule type="expression" dxfId="40" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="15">
+    <cfRule type="expression" dxfId="36" priority="15">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D60">
-    <cfRule type="expression" dxfId="38" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="14">
+    <cfRule type="expression" dxfId="34" priority="14">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E60">
-    <cfRule type="expression" dxfId="36" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F60">
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F60">
-    <cfRule type="expression" dxfId="32" priority="12">
+    <cfRule type="expression" dxfId="29" priority="12">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="17" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G60">
-    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H60">
-    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I60">
-    <cfRule type="expression" dxfId="26" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J60">
-    <cfRule type="cellIs" dxfId="24" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J60">
-    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
v0.1.9 - Updated admin report amounts
</commit_message>
<xml_diff>
--- a/administrador/resumen_general.xlsx
+++ b/administrador/resumen_general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/administrador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8163DCCA-D7B4-584C-8378-98534862C8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0820E68-4E4A-7F47-AFAD-00AE5016E189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16360" xr2:uid="{0B03E385-4D70-1443-97FA-03D8B48AE23F}"/>
   </bookViews>
@@ -755,241 +755,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="152">
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="134">
     <dxf>
       <border>
         <left style="hair">
@@ -3184,57 +2950,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:F47" totalsRowShown="0" headerRowDxfId="151" dataDxfId="149" headerRowBorderDxfId="150" tableBorderDxfId="148">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:F47" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130">
   <autoFilter ref="A2:F47" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="146"/>
-    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas_Pagado" dataDxfId="145"/>
-    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Total_Pagado" dataDxfId="144"/>
-    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Pólizas_Pendiente" dataDxfId="143"/>
-    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Total_Pendiente" dataDxfId="142"/>
+    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="129"/>
+    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="128"/>
+    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas_Pagado" dataDxfId="127"/>
+    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Total_Pagado" dataDxfId="126"/>
+    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Pólizas_Pendiente" dataDxfId="125"/>
+    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Total_Pendiente" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="N2:Y6" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="139"/>
-    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="138"/>
-    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="137" dataCellStyle="Porcentaje"/>
-    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="136" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="135" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="134" dataCellStyle="Porcentaje"/>
-    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="133" dataCellStyle="Porcentaje"/>
-    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="132" dataCellStyle="Porcentaje"/>
-    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="131" dataCellStyle="Porcentaje"/>
-    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="130" dataCellStyle="Porcentaje"/>
-    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="129"/>
-    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="128"/>
+    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="119" dataCellStyle="Porcentaje"/>
+    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="118" dataCellStyle="Porcentaje"/>
+    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="117" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="116" dataCellStyle="Porcentaje"/>
+    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="115" dataCellStyle="Porcentaje"/>
+    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="114" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="113" dataCellStyle="Porcentaje"/>
+    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="112" dataCellStyle="Porcentaje"/>
+    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="111"/>
+    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
   <autoFilter ref="A2:L49" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="121"/>
-    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="120"/>
-    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="119"/>
-    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="118"/>
-    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="117"/>
-    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="116"/>
-    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="115"/>
-    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="102"/>
+    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="101"/>
+    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="100"/>
+    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="99"/>
+    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="98"/>
+    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="97"/>
+    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3259,26 +3025,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A2:J60" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="111"/>
-    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="107"/>
-    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="106" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="105"/>
-    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="104"/>
-    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="103"/>
-    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="102" dataCellStyle="Porcentaje"/>
+    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="93"/>
+    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="88" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="84" dataCellStyle="Porcentaje"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="101" headerRowBorderDxfId="100" tableBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="M2:AB4" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{092EDBAB-8D8A-EA4D-9E0C-E48510EA1510}" name="Polizas_Pagadas_Año_Anterior"/>
@@ -3625,7 +3391,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3789,10 +3555,10 @@
         <v>27079.33</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>801637.94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -4565,114 +4331,114 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="expression" dxfId="80" priority="18" stopIfTrue="1">
+      <formula>$S$34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A46">
+    <cfRule type="expression" dxfId="79" priority="17" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="16" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="95" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="71" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="70" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="75" priority="15" stopIfTrue="1">
+      <formula>$S$34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B46">
+    <cfRule type="expression" dxfId="74" priority="13" stopIfTrue="1">
+      <formula>$S4=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="14" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="90" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="74" stopIfTrue="1">
       <formula>$Q95=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="73" stopIfTrue="1">
       <formula>$Q96=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:D47 F47">
-    <cfRule type="expression" dxfId="88" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="91" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="77" priority="89" stopIfTrue="1">
-      <formula>$Q47=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="90" stopIfTrue="1">
-      <formula>$Q46=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A46">
-    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+  <conditionalFormatting sqref="C3">
+    <cfRule type="expression" dxfId="68" priority="12" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
-      <formula>$S$34=1</formula>
+  <conditionalFormatting sqref="C4:C46">
+    <cfRule type="expression" dxfId="67" priority="11" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="10" stopIfTrue="1">
+      <formula>$S4=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B46">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C46">
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+  <conditionalFormatting sqref="D3">
+    <cfRule type="expression" dxfId="65" priority="9" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D46">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="8" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="7" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>$S3=1</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="62" priority="6" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E46">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="5" stopIfTrue="1">
+      <formula>$S3=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="4" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>$S3=1</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" dxfId="59" priority="89" stopIfTrue="1">
+      <formula>$Q47=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="90" stopIfTrue="1">
+      <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+  <conditionalFormatting sqref="F3">
+    <cfRule type="expression" dxfId="57" priority="3" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F46">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
-      <formula>$S4=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="2" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>$S$34=1</formula>
+    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
+      <formula>$S4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6588,145 +6354,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A49">
-    <cfRule type="expression" dxfId="72" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="19" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B49">
-    <cfRule type="expression" dxfId="70" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="16" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="17" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C49">
-    <cfRule type="expression" dxfId="68" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="12" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:H49">
-    <cfRule type="expression" dxfId="67" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="13" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D49">
-    <cfRule type="expression" dxfId="66" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="11" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E49">
-    <cfRule type="expression" dxfId="65" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="10" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F49">
-    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G49">
-    <cfRule type="expression" dxfId="63" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H49">
-    <cfRule type="expression" dxfId="62" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I49">
-    <cfRule type="expression" dxfId="61" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
       <formula>$R3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="14" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J49">
-    <cfRule type="expression" dxfId="59" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="2" stopIfTrue="1">
       <formula>$S3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K49">
-    <cfRule type="expression" dxfId="57" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="3" stopIfTrue="1">
       <formula>$T3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L49">
-    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="1" stopIfTrue="1">
       <formula>$U3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="4" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N6">
-    <cfRule type="expression" dxfId="53" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O6">
-    <cfRule type="expression" dxfId="52" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="30" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P6">
-    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="29" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q6">
-    <cfRule type="expression" dxfId="50" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="28" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R6">
-    <cfRule type="expression" dxfId="49" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="27" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S6">
-    <cfRule type="expression" dxfId="48" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="26" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T6">
-    <cfRule type="expression" dxfId="47" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U6">
-    <cfRule type="expression" dxfId="46" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V6">
-    <cfRule type="expression" dxfId="45" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="23" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W6">
-    <cfRule type="expression" dxfId="44" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X6">
-    <cfRule type="expression" dxfId="43" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="21" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y6">
-    <cfRule type="expression" dxfId="42" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10235,98 +10001,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A60">
-    <cfRule type="expression" dxfId="41" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="expression" dxfId="39" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C60">
-    <cfRule type="expression" dxfId="37" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D60">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E60">
-    <cfRule type="expression" dxfId="33" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F60">
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F60">
-    <cfRule type="expression" dxfId="29" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G60">
-    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H60">
-    <cfRule type="expression" dxfId="25" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I60">
-    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J60">
-    <cfRule type="cellIs" dxfId="21" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J60">
-    <cfRule type="expression" dxfId="19" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
v0.2.3 - Updated Pagado/Pendiente data (Feb 25 cut-off)
</commit_message>
<xml_diff>
--- a/administrador/resumen_general.xlsx
+++ b/administrador/resumen_general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/panel de campañas/administrador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E229FD-562A-2B49-B320-C4C2F5097901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814158B0-4173-5D45-9782-228891D97BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0B03E385-4D70-1443-97FA-03D8B48AE23F}"/>
   </bookViews>
@@ -765,7 +765,303 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="166">
+  <dxfs count="189">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
@@ -3398,61 +3694,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:J47" totalsRowShown="0" headerRowDxfId="165" dataDxfId="163" headerRowBorderDxfId="164" tableBorderDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}" name="Tabla2" displayName="Tabla2" ref="A2:J47" totalsRowShown="0" headerRowDxfId="188" dataDxfId="186" headerRowBorderDxfId="187" tableBorderDxfId="185">
   <autoFilter ref="A2:J47" xr:uid="{EF3678E2-D2A6-8844-A43D-E5D3D290BCA5}"/>
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="160"/>
-    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas-Pagadas" dataDxfId="159"/>
-    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Recibo_Inicial_Pagado" dataDxfId="158"/>
-    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Recibo_Ordinario_Pagado" dataDxfId="157"/>
-    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Total _Prima_Pagada" dataDxfId="156"/>
-    <tableColumn id="1" xr3:uid="{E28A327A-321D-AB4B-A3E4-B84B36B11129}" name="Pólizas_Pendinetes" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{2AAC82E1-6CC3-F045-B587-E5A490F632BF}" name="Recibo_Inicial_Pendiente" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{1857825C-6430-7844-B09E-A33AFAEE6854}" name="Recibo_Ordinario_Pendiente" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{48B56B42-A49D-2E42-8271-5CB59AB26C60}" name="Total _Prima_Pendiente" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{567489A3-0130-DE4E-B66F-770D47C320B3}" name="Nombre Asesor" dataDxfId="184"/>
+    <tableColumn id="3" xr3:uid="{6065379F-3C87-B349-8B0F-6362B9908C0D}" name="Sucursal" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{DFDB0618-8825-D24B-BE4F-C2CBA1EB5FDC}" name="Pólizas-Pagadas" dataDxfId="182"/>
+    <tableColumn id="6" xr3:uid="{6E4EF166-CCB0-5B4D-B02F-98DED29DC247}" name="Recibo_Inicial_Pagado" dataDxfId="181"/>
+    <tableColumn id="7" xr3:uid="{756B903A-962E-F640-B6D0-43B46DBAE2C4}" name="Recibo_Ordinario_Pagado" dataDxfId="180"/>
+    <tableColumn id="8" xr3:uid="{15464F8D-A190-224E-954A-B011EC99914E}" name="Total _Prima_Pagada" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{E28A327A-321D-AB4B-A3E4-B84B36B11129}" name="Pólizas_Pendinetes" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{2AAC82E1-6CC3-F045-B587-E5A490F632BF}" name="Recibo_Inicial_Pendiente" dataDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{1857825C-6430-7844-B09E-A33AFAEE6854}" name="Recibo_Ordinario_Pendiente" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{48B56B42-A49D-2E42-8271-5CB59AB26C60}" name="Total _Prima_Pendiente" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}" name="Tabla3" displayName="Tabla3" ref="N2:Y6" totalsRowShown="0" headerRowDxfId="178" dataDxfId="177">
   <autoFilter ref="N2:Y6" xr:uid="{C7996A95-CF3C-F141-8E91-B8BCC568AE96}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="153"/>
-    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="152"/>
-    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="151" dataCellStyle="Porcentaje"/>
-    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="150" dataCellStyle="Porcentaje"/>
-    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="149" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="148" dataCellStyle="Porcentaje"/>
-    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="147" dataCellStyle="Porcentaje"/>
-    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="146" dataCellStyle="Porcentaje"/>
-    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="145" dataCellStyle="Porcentaje"/>
-    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="144" dataCellStyle="Porcentaje"/>
-    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="143"/>
-    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="142"/>
+    <tableColumn id="1" xr3:uid="{2C62924E-321A-3F41-AF78-C7BD48702FE6}" name="Sucursal" dataDxfId="176"/>
+    <tableColumn id="2" xr3:uid="{03EE0001-075B-DB48-BD6C-FD285343B8DF}" name="Agentes" dataDxfId="175"/>
+    <tableColumn id="3" xr3:uid="{D322F0A9-DF1B-6342-A752-2BD474FD8932}" name="Asesores_con_Emisión_Vida" dataDxfId="174" dataCellStyle="Porcentaje"/>
+    <tableColumn id="4" xr3:uid="{89CC3B21-F460-AF40-88BA-662B3F86DD2F}" name="%_Asesores_con_Emisión_Vida" dataDxfId="173" dataCellStyle="Porcentaje"/>
+    <tableColumn id="5" xr3:uid="{AEA4345E-12E1-5041-8E34-03CD029CF4C8}" name="Asesores_con_Emisión_GMM" dataDxfId="172" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{A33DEBAA-81E1-5745-809D-3225F616DE15}" name="%_Asesores_con_Emisión_GMM" dataDxfId="171" dataCellStyle="Porcentaje"/>
+    <tableColumn id="7" xr3:uid="{E547A12E-38A5-3645-9DE2-EFF3DCF3DB30}" name="Asesores_con_pol_Pagada_Vida" dataDxfId="170" dataCellStyle="Porcentaje"/>
+    <tableColumn id="8" xr3:uid="{D5C38221-7805-B14F-ACF8-6D63156AA187}" name="%_Asesores_con_pol_Pagada_Vida" dataDxfId="169" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{236C76F2-7149-8148-9FE3-6C51C2181E13}" name="Asesores_con_pol_Pagada_GMM" dataDxfId="168" dataCellStyle="Porcentaje"/>
+    <tableColumn id="10" xr3:uid="{23DD5D1F-6EF8-E44C-A7A9-67C308D41B1B}" name="%_Asesores_con_pol_Pagada_GMM" dataDxfId="167" dataCellStyle="Porcentaje"/>
+    <tableColumn id="11" xr3:uid="{D3D66AF9-B8A7-DF4D-BBD1-7727B28B50BB}" name="Prima_Pagada_Vida" dataDxfId="166"/>
+    <tableColumn id="12" xr3:uid="{BCF3339C-535D-7143-87C3-088A311729F3}" name="Prima_Pagada_GMM" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}" name="Tabla7" displayName="Tabla7" ref="A2:L49" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163">
   <autoFilter ref="A2:L49" xr:uid="{95F6C6AD-0F36-4543-B787-C113356A3C91}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="139"/>
-    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="137"/>
-    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="136"/>
-    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="135"/>
-    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="134"/>
-    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="133"/>
-    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="132"/>
-    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="131"/>
-    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="130"/>
-    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="129"/>
-    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="128"/>
+    <tableColumn id="1" xr3:uid="{2204DBA5-0702-1245-99CF-F40C8C6E52B6}" name="Asesor" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{BC529EE2-4C82-9A4F-8611-5361D795A324}" name="Sucursal" dataDxfId="161"/>
+    <tableColumn id="4" xr3:uid="{1E32D02E-886A-7F4F-A030-020603C42B62}" name="Emitido_Vida" dataDxfId="160"/>
+    <tableColumn id="5" xr3:uid="{90E38267-9AAC-6C4E-89C4-6FD642480CE9}" name="Emitido_GMM" dataDxfId="159"/>
+    <tableColumn id="6" xr3:uid="{04B64085-4C47-B349-B80C-94CC79537BBF}" name="Pagado_Vida" dataDxfId="158"/>
+    <tableColumn id="7" xr3:uid="{8B103651-A253-DC4C-AA6B-8797B74ED794}" name="Pagado_GMM" dataDxfId="157"/>
+    <tableColumn id="8" xr3:uid="{5942D024-C75F-9347-A784-5F257195BF6B}" name="Prima_Pagada_Vida" dataDxfId="156"/>
+    <tableColumn id="9" xr3:uid="{7D199811-1CC4-2C41-A6AF-44138B23B1AA}" name="Prima_Pagada_GMM" dataDxfId="155"/>
+    <tableColumn id="10" xr3:uid="{40107B60-D100-674B-900D-B96E19CFFA25}" name="Sin_Emisión_Vida" dataDxfId="154"/>
+    <tableColumn id="11" xr3:uid="{4B6995EB-7B42-7240-9BA4-85136CA6F418}" name="Sin_Emisión_GMM" dataDxfId="153"/>
+    <tableColumn id="12" xr3:uid="{A089BD91-0F49-8A40-922D-B82A9DA46E38}" name="3_Meses_Sin_Emisión_Vida" dataDxfId="152"/>
+    <tableColumn id="13" xr3:uid="{F02A0105-00B0-734A-B20B-31E07B82908D}" name="3_Meses_Sin_Emisión_GMM" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3477,26 +3773,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}" name="Tabla8" displayName="Tabla8" ref="A2:J60" totalsRowShown="0" headerRowDxfId="150" dataDxfId="149">
   <autoFilter ref="A2:J60" xr:uid="{8E304F4B-C1E2-9E4A-98A7-5782F07B324B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="125"/>
-    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="123"/>
-    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="122"/>
-    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="121"/>
-    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="120" dataCellStyle="Porcentaje"/>
-    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="118"/>
-    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="117"/>
-    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="116" dataCellStyle="Porcentaje"/>
+    <tableColumn id="1" xr3:uid="{D83FB5D5-E48D-CC46-830D-D387CDA99429}" name="Asesor" dataDxfId="148"/>
+    <tableColumn id="10" xr3:uid="{C470ED6D-1901-E740-A398-E6BD65F8E6AF}" name="Sucursal" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{BFC0EA40-E0A9-E94E-9D8A-75B738703021}" name="Polizas_Pagadas_Año_Anterior" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{892529B2-ABAE-EF44-8537-4418F64F171B}" name="Polizas_Pagadas_Año_Actual" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{2F379D17-28E1-B240-AAD1-AAFAD4060ADB}" name="Crec_Polizas_Pagadas" dataDxfId="144"/>
+    <tableColumn id="5" xr3:uid="{45011D63-A532-9142-BF79-165C02039C51}" name="%_Crec_Polizas_Pagadas" dataDxfId="143" dataCellStyle="Porcentaje"/>
+    <tableColumn id="6" xr3:uid="{F115372D-3BF6-F54E-B2F9-27E216A48542}" name="Prima_Pagada_Año_Anterior" dataDxfId="142"/>
+    <tableColumn id="7" xr3:uid="{566C8A2B-6902-1449-BDEA-34F00E69779A}" name="Prima_Pagada_Año_Actual" dataDxfId="141"/>
+    <tableColumn id="8" xr3:uid="{7C5D56D7-9B6D-C64F-A643-94A7B3FCAC39}" name="Crec_Prima_Pagada" dataDxfId="140"/>
+    <tableColumn id="9" xr3:uid="{0DFBD021-0FCA-0748-839C-22C72DCBA35F}" name="%_Crec_Prima_Pagada" dataDxfId="139" dataCellStyle="Porcentaje"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="115" headerRowBorderDxfId="114" tableBorderDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}" name="Tabla10" displayName="Tabla10" ref="M2:AB4" totalsRowShown="0" headerRowDxfId="138" headerRowBorderDxfId="137" tableBorderDxfId="136">
   <autoFilter ref="M2:AB4" xr:uid="{A29DCA76-5097-2F45-94DA-4B121F22F1F5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{092EDBAB-8D8A-EA4D-9E0C-E48510EA1510}" name="Polizas_Pagadas_Año_Anterior"/>
@@ -3843,7 +4139,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3862,7 +4158,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="34">
-        <v>46077</v>
+        <v>46078</v>
       </c>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -3947,10 +4243,10 @@
         <v>2979.51</v>
       </c>
       <c r="E4" s="4">
-        <v>111205.27</v>
+        <v>116582.82</v>
       </c>
       <c r="F4" s="4">
-        <v>114184.78</v>
+        <v>119562.33</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -3959,10 +4255,10 @@
         <v>24118.68</v>
       </c>
       <c r="I4" s="4">
-        <v>251326.53</v>
+        <v>245948.98</v>
       </c>
       <c r="J4" s="4">
-        <v>275445.21000000002</v>
+        <v>270067.65999999997</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -3999,86 +4295,86 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>2856</v>
       </c>
       <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>18550.03</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36422.839999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>54972.87</v>
+      </c>
+      <c r="G6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
-        <v>3273.67</v>
-      </c>
-      <c r="E6" s="4">
-        <v>49709.32</v>
-      </c>
-      <c r="F6" s="4">
-        <v>52982.99</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
       <c r="H6" s="4">
-        <v>0</v>
+        <v>3698.6</v>
       </c>
       <c r="I6" s="4">
-        <v>21966.880000000001</v>
+        <v>189775.73</v>
       </c>
       <c r="J6" s="4">
-        <v>21966.880000000001</v>
+        <v>193474.33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2">
         <v>2856</v>
       </c>
       <c r="C7" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="4">
-        <v>18550.03</v>
+        <v>3273.67</v>
       </c>
       <c r="E7" s="4">
-        <v>33725.25</v>
+        <v>49709.32</v>
       </c>
       <c r="F7" s="4">
-        <v>52275.28</v>
+        <v>52982.99</v>
       </c>
       <c r="G7" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>3698.6</v>
+        <v>0</v>
       </c>
       <c r="I7" s="4">
-        <v>189775.73</v>
+        <v>21966.880000000001</v>
       </c>
       <c r="J7" s="4">
-        <v>193474.33</v>
+        <v>21966.880000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>2692</v>
       </c>
       <c r="C8" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>8771.2099999999991</v>
+        <v>1657.5</v>
       </c>
       <c r="E8" s="4">
-        <v>25352.99</v>
+        <v>41014.769999999997</v>
       </c>
       <c r="F8" s="4">
-        <v>34124.199999999997</v>
+        <v>42672.27</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -4087,30 +4383,30 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <v>114458.92</v>
+        <v>50354.53</v>
       </c>
       <c r="J8" s="4">
-        <v>114458.92</v>
+        <v>50354.53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="4">
-        <v>0</v>
+        <v>8771.2099999999991</v>
       </c>
       <c r="E9" s="4">
-        <v>27079.33</v>
+        <v>25352.99</v>
       </c>
       <c r="F9" s="4">
-        <v>27079.33</v>
+        <v>34124.199999999997</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -4119,15 +4415,15 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <v>129008.51</v>
+        <v>114458.92</v>
       </c>
       <c r="J9" s="4">
-        <v>129008.51</v>
+        <v>114458.92</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>2043</v>
@@ -4139,94 +4435,94 @@
         <v>0</v>
       </c>
       <c r="E10" s="4">
-        <v>22054.400000000001</v>
+        <v>27079.33</v>
       </c>
       <c r="F10" s="4">
-        <v>22054.400000000001</v>
+        <v>27079.33</v>
       </c>
       <c r="G10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
-        <v>24026.04</v>
+        <v>0</v>
       </c>
       <c r="I10" s="4">
-        <v>75875.25</v>
+        <v>129008.51</v>
       </c>
       <c r="J10" s="4">
-        <v>99901.29</v>
+        <v>129008.51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>2856</v>
+        <v>2692</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>11621.35</v>
       </c>
       <c r="E11" s="4">
-        <v>20077.400000000001</v>
+        <v>11532.26</v>
       </c>
       <c r="F11" s="4">
-        <v>20077.400000000001</v>
+        <v>23153.61</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
-        <v>0</v>
+        <v>10311.540000000001</v>
       </c>
       <c r="I11" s="4">
-        <v>42810.25</v>
+        <v>37026.089999999997</v>
       </c>
       <c r="J11" s="4">
-        <v>42810.25</v>
+        <v>47337.63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2">
         <v>2043</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>1973.29</v>
+        <v>0</v>
       </c>
       <c r="E12" s="4">
-        <v>13552</v>
+        <v>22054.400000000001</v>
       </c>
       <c r="F12" s="4">
-        <v>15525.29</v>
+        <v>22054.400000000001</v>
       </c>
       <c r="G12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="4">
-        <v>0</v>
+        <v>24026.04</v>
       </c>
       <c r="I12" s="4">
-        <v>46859.360000000001</v>
+        <v>75875.25</v>
       </c>
       <c r="J12" s="4">
-        <v>46859.360000000001</v>
+        <v>99901.29</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -4235,10 +4531,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="4">
-        <v>14887.38</v>
+        <v>20077.400000000001</v>
       </c>
       <c r="F13" s="4">
-        <v>14887.38</v>
+        <v>20077.400000000001</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -4247,30 +4543,30 @@
         <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>14887.38</v>
+        <v>42810.25</v>
       </c>
       <c r="J13" s="4">
-        <v>14887.38</v>
+        <v>42810.25</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="4">
-        <v>0</v>
+        <v>1973.29</v>
       </c>
       <c r="E14" s="4">
-        <v>14217.61</v>
+        <v>13552</v>
       </c>
       <c r="F14" s="4">
-        <v>14217.61</v>
+        <v>15525.29</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -4279,18 +4575,18 @@
         <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>113740.88</v>
+        <v>46859.360000000001</v>
       </c>
       <c r="J14" s="4">
-        <v>113740.88</v>
+        <v>46859.360000000001</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -4299,10 +4595,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="4">
-        <v>11945.29</v>
+        <v>14887.38</v>
       </c>
       <c r="F15" s="4">
-        <v>11945.29</v>
+        <v>14887.38</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
@@ -4311,15 +4607,15 @@
         <v>0</v>
       </c>
       <c r="I15" s="4">
-        <v>66315.25</v>
+        <v>14887.38</v>
       </c>
       <c r="J15" s="4">
-        <v>66315.25</v>
+        <v>14887.38</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2">
         <v>2692</v>
@@ -4331,30 +4627,30 @@
         <v>0</v>
       </c>
       <c r="E16" s="4">
-        <v>11532.26</v>
+        <v>14217.61</v>
       </c>
       <c r="F16" s="4">
-        <v>11532.26</v>
+        <v>14217.61</v>
       </c>
       <c r="G16" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4">
-        <v>21932.89</v>
+        <v>0</v>
       </c>
       <c r="I16" s="4">
-        <v>37026.089999999997</v>
+        <v>113740.88</v>
       </c>
       <c r="J16" s="4">
-        <v>58958.98</v>
+        <v>113740.88</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -4363,10 +4659,10 @@
         <v>0</v>
       </c>
       <c r="E17" s="4">
-        <v>9688.8700000000008</v>
+        <v>11945.29</v>
       </c>
       <c r="F17" s="4">
-        <v>9688.8700000000008</v>
+        <v>11945.29</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -4375,10 +4671,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="4">
-        <v>24855.21</v>
+        <v>66315.25</v>
       </c>
       <c r="J17" s="4">
-        <v>24855.21</v>
+        <v>66315.25</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -4395,10 +4691,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="4">
-        <v>9281.48</v>
+        <v>10995.07</v>
       </c>
       <c r="F18" s="4">
-        <v>9281.48</v>
+        <v>10995.07</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -4407,15 +4703,15 @@
         <v>0</v>
       </c>
       <c r="I18" s="4">
-        <v>34668.69</v>
+        <v>32955.1</v>
       </c>
       <c r="J18" s="4">
-        <v>34668.69</v>
+        <v>32955.1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2">
         <v>2043</v>
@@ -4427,10 +4723,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="4">
-        <v>8821.32</v>
+        <v>9688.8700000000008</v>
       </c>
       <c r="F19" s="4">
-        <v>8821.32</v>
+        <v>9688.8700000000008</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -4439,18 +4735,18 @@
         <v>0</v>
       </c>
       <c r="I19" s="4">
-        <v>11272.92</v>
+        <v>24855.21</v>
       </c>
       <c r="J19" s="4">
-        <v>11272.92</v>
+        <v>24855.21</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -4459,10 +4755,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="4">
-        <v>7991.52</v>
+        <v>8821.32</v>
       </c>
       <c r="F20" s="4">
-        <v>7991.52</v>
+        <v>8821.32</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -4471,15 +4767,15 @@
         <v>0</v>
       </c>
       <c r="I20" s="4">
-        <v>55306.96</v>
+        <v>11272.92</v>
       </c>
       <c r="J20" s="4">
-        <v>55306.96</v>
+        <v>11272.92</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2">
         <v>2692</v>
@@ -4488,13 +4784,13 @@
         <v>0</v>
       </c>
       <c r="D21" s="4">
-        <v>-6.95</v>
+        <v>0</v>
       </c>
       <c r="E21" s="4">
-        <v>7467.79</v>
+        <v>7991.52</v>
       </c>
       <c r="F21" s="4">
-        <v>7460.84</v>
+        <v>7991.52</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
@@ -4503,30 +4799,30 @@
         <v>0</v>
       </c>
       <c r="I21" s="4">
-        <v>15352.07</v>
+        <v>55306.96</v>
       </c>
       <c r="J21" s="4">
-        <v>15352.07</v>
+        <v>55306.96</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2">
-        <v>2856</v>
+        <v>2692</v>
       </c>
       <c r="C22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>1809.19</v>
+        <v>-6.95</v>
       </c>
       <c r="E22" s="4">
-        <v>4906.95</v>
+        <v>7467.79</v>
       </c>
       <c r="F22" s="4">
-        <v>6716.14</v>
+        <v>7460.84</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
@@ -4535,30 +4831,30 @@
         <v>0</v>
       </c>
       <c r="I22" s="4">
-        <v>43873.2</v>
+        <v>15352.07</v>
       </c>
       <c r="J22" s="4">
-        <v>43873.2</v>
+        <v>15352.07</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="4">
-        <v>0</v>
+        <v>2300.5300000000002</v>
       </c>
       <c r="E23" s="4">
-        <v>6639.64</v>
+        <v>4417.25</v>
       </c>
       <c r="F23" s="4">
-        <v>6639.64</v>
+        <v>6717.78</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
@@ -4567,30 +4863,30 @@
         <v>0</v>
       </c>
       <c r="I23" s="4">
-        <v>8336.92</v>
+        <v>0</v>
       </c>
       <c r="J23" s="4">
-        <v>8336.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2">
-        <v>2692</v>
+        <v>2856</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
+        <v>1809.19</v>
       </c>
       <c r="E24" s="4">
-        <v>6463.82</v>
+        <v>4906.95</v>
       </c>
       <c r="F24" s="4">
-        <v>6463.82</v>
+        <v>6716.14</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
@@ -4599,18 +4895,18 @@
         <v>0</v>
       </c>
       <c r="I24" s="4">
-        <v>60745.99</v>
+        <v>43873.2</v>
       </c>
       <c r="J24" s="4">
-        <v>60745.99</v>
+        <v>43873.2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -4619,10 +4915,10 @@
         <v>0</v>
       </c>
       <c r="E25" s="4">
-        <v>6196.74</v>
+        <v>6639.64</v>
       </c>
       <c r="F25" s="4">
-        <v>6196.74</v>
+        <v>6639.64</v>
       </c>
       <c r="G25" s="3">
         <v>0</v>
@@ -4631,18 +4927,18 @@
         <v>0</v>
       </c>
       <c r="I25" s="4">
-        <v>0</v>
+        <v>8336.92</v>
       </c>
       <c r="J25" s="4">
-        <v>0</v>
+        <v>8336.92</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2">
-        <v>2043</v>
+        <v>2692</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -4651,10 +4947,10 @@
         <v>0</v>
       </c>
       <c r="E26" s="4">
-        <v>6125.03</v>
+        <v>6463.82</v>
       </c>
       <c r="F26" s="4">
-        <v>6125.03</v>
+        <v>6463.82</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
@@ -4663,18 +4959,18 @@
         <v>0</v>
       </c>
       <c r="I26" s="4">
-        <v>0</v>
+        <v>60745.99</v>
       </c>
       <c r="J26" s="4">
-        <v>0</v>
+        <v>60745.99</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2">
-        <v>2692</v>
+        <v>2043</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -4683,27 +4979,27 @@
         <v>0</v>
       </c>
       <c r="E27" s="4">
-        <v>5895.02</v>
+        <v>6196.74</v>
       </c>
       <c r="F27" s="4">
-        <v>5895.02</v>
+        <v>6196.74</v>
       </c>
       <c r="G27" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="4">
-        <v>36777.25</v>
+        <v>0</v>
       </c>
       <c r="I27" s="4">
-        <v>50354.53</v>
+        <v>0</v>
       </c>
       <c r="J27" s="4">
-        <v>87131.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2">
         <v>2043</v>
@@ -4715,10 +5011,10 @@
         <v>0</v>
       </c>
       <c r="E28" s="4">
-        <v>5745.69</v>
+        <v>6125.03</v>
       </c>
       <c r="F28" s="4">
-        <v>5745.69</v>
+        <v>6125.03</v>
       </c>
       <c r="G28" s="3">
         <v>0</v>
@@ -4727,15 +5023,15 @@
         <v>0</v>
       </c>
       <c r="I28" s="4">
-        <v>22496</v>
+        <v>0</v>
       </c>
       <c r="J28" s="4">
-        <v>22496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B29" s="2">
         <v>2043</v>
@@ -4747,27 +5043,27 @@
         <v>0</v>
       </c>
       <c r="E29" s="4">
-        <v>5620.13</v>
+        <v>5745.69</v>
       </c>
       <c r="F29" s="4">
-        <v>5620.13</v>
+        <v>5745.69</v>
       </c>
       <c r="G29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4">
-        <v>24131.27</v>
+        <v>0</v>
       </c>
       <c r="I29" s="4">
-        <v>23573.33</v>
+        <v>22496</v>
       </c>
       <c r="J29" s="4">
-        <v>47704.6</v>
+        <v>22496</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B30" s="2">
         <v>2043</v>
@@ -4779,27 +5075,27 @@
         <v>0</v>
       </c>
       <c r="E30" s="4">
-        <v>5138.51</v>
+        <v>5620.13</v>
       </c>
       <c r="F30" s="4">
-        <v>5138.51</v>
+        <v>5620.13</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="4">
-        <v>0</v>
+        <v>24131.27</v>
       </c>
       <c r="I30" s="4">
-        <v>10277.030000000001</v>
+        <v>23573.33</v>
       </c>
       <c r="J30" s="4">
-        <v>10277.030000000001</v>
+        <v>47704.6</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2">
         <v>2043</v>
@@ -4811,10 +5107,10 @@
         <v>0</v>
       </c>
       <c r="E31" s="4">
-        <v>5089.54</v>
+        <v>5138.51</v>
       </c>
       <c r="F31" s="4">
-        <v>5089.54</v>
+        <v>5138.51</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -4823,15 +5119,15 @@
         <v>0</v>
       </c>
       <c r="I31" s="4">
-        <v>10679.89</v>
+        <v>10277.030000000001</v>
       </c>
       <c r="J31" s="4">
-        <v>10679.89</v>
+        <v>10277.030000000001</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B32" s="2">
         <v>2043</v>
@@ -4843,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="E32" s="4">
-        <v>4663.49</v>
+        <v>5089.54</v>
       </c>
       <c r="F32" s="4">
-        <v>4663.49</v>
+        <v>5089.54</v>
       </c>
       <c r="G32" s="3">
         <v>0</v>
@@ -4855,18 +5151,18 @@
         <v>0</v>
       </c>
       <c r="I32" s="4">
-        <v>3167.47</v>
+        <v>5098.3999999999996</v>
       </c>
       <c r="J32" s="4">
-        <v>3167.47</v>
+        <v>5098.3999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
@@ -4875,10 +5171,10 @@
         <v>0</v>
       </c>
       <c r="E33" s="4">
-        <v>4487.59</v>
+        <v>4663.49</v>
       </c>
       <c r="F33" s="4">
-        <v>4487.59</v>
+        <v>4663.49</v>
       </c>
       <c r="G33" s="3">
         <v>0</v>
@@ -4887,18 +5183,18 @@
         <v>0</v>
       </c>
       <c r="I33" s="4">
-        <v>38209.879999999997</v>
+        <v>3167.47</v>
       </c>
       <c r="J33" s="4">
-        <v>38209.879999999997</v>
+        <v>3167.47</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B34" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -4907,10 +5203,10 @@
         <v>0</v>
       </c>
       <c r="E34" s="4">
-        <v>4192.72</v>
+        <v>4487.59</v>
       </c>
       <c r="F34" s="4">
-        <v>4192.72</v>
+        <v>4487.59</v>
       </c>
       <c r="G34" s="3">
         <v>0</v>
@@ -4919,79 +5215,79 @@
         <v>0</v>
       </c>
       <c r="I34" s="4">
-        <v>23946.42</v>
+        <v>38209.879999999997</v>
       </c>
       <c r="J34" s="4">
-        <v>23946.42</v>
+        <v>38209.879999999997</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2">
-        <v>2856</v>
+        <v>2043</v>
       </c>
       <c r="C35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>2561.44</v>
+        <v>0</v>
       </c>
       <c r="E35" s="4">
-        <v>1432.54</v>
+        <v>4192.72</v>
       </c>
       <c r="F35" s="4">
-        <v>3993.98</v>
+        <v>4192.72</v>
       </c>
       <c r="G35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="4">
-        <v>5165.8599999999997</v>
+        <v>0</v>
       </c>
       <c r="I35" s="4">
-        <v>21373.95</v>
+        <v>23946.42</v>
       </c>
       <c r="J35" s="4">
-        <v>26539.81</v>
+        <v>23946.42</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B36" s="2">
-        <v>2043</v>
+        <v>2856</v>
       </c>
       <c r="C36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>2561.44</v>
       </c>
       <c r="E36" s="4">
-        <v>3151.08</v>
+        <v>1432.54</v>
       </c>
       <c r="F36" s="4">
-        <v>3151.08</v>
+        <v>3993.98</v>
       </c>
       <c r="G36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="4">
-        <v>0</v>
+        <v>5165.8599999999997</v>
       </c>
       <c r="I36" s="4">
-        <v>0</v>
+        <v>21373.95</v>
       </c>
       <c r="J36" s="4">
-        <v>0</v>
+        <v>26539.81</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B37" s="2">
         <v>2043</v>
@@ -5003,10 +5299,10 @@
         <v>0</v>
       </c>
       <c r="E37" s="4">
-        <v>2852.69</v>
+        <v>3151.08</v>
       </c>
       <c r="F37" s="4">
-        <v>2852.69</v>
+        <v>3151.08</v>
       </c>
       <c r="G37" s="3">
         <v>0</v>
@@ -5015,15 +5311,15 @@
         <v>0</v>
       </c>
       <c r="I37" s="4">
-        <v>1575.88</v>
+        <v>0</v>
       </c>
       <c r="J37" s="4">
-        <v>1575.88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2">
         <v>2043</v>
@@ -5035,10 +5331,10 @@
         <v>0</v>
       </c>
       <c r="E38" s="4">
-        <v>2833.03</v>
+        <v>2852.69</v>
       </c>
       <c r="F38" s="4">
-        <v>2833.03</v>
+        <v>2852.69</v>
       </c>
       <c r="G38" s="3">
         <v>0</v>
@@ -5047,15 +5343,15 @@
         <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>4506.84</v>
+        <v>1575.88</v>
       </c>
       <c r="J38" s="4">
-        <v>4506.84</v>
+        <v>1575.88</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2">
         <v>2043</v>
@@ -5067,22 +5363,22 @@
         <v>0</v>
       </c>
       <c r="E39" s="4">
-        <v>2133.91</v>
+        <v>2833.03</v>
       </c>
       <c r="F39" s="4">
-        <v>2133.91</v>
+        <v>2833.03</v>
       </c>
       <c r="G39" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="4">
-        <v>5102.97</v>
+        <v>0</v>
       </c>
       <c r="I39" s="4">
-        <v>0</v>
+        <v>4506.84</v>
       </c>
       <c r="J39" s="4">
-        <v>5102.97</v>
+        <v>4506.84</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -5324,60 +5620,60 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="109" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="122" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="121" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="104" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="125" stopIfTrue="1">
       <formula>$Q95=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="124" stopIfTrue="1">
       <formula>$Q96=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:D47 F47">
-    <cfRule type="expression" dxfId="102" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="143" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="119" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="142" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="91" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="140" stopIfTrue="1">
       <formula>$Q47=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="141" stopIfTrue="1">
       <formula>$Q46=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A46">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="21" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B46">
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5397,7 +5693,7 @@
       <formula>$S3=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F46 J4:J8 J10:J46">
+  <conditionalFormatting sqref="F4:F46 J4:J9 J11:J46">
     <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>$S4=1</formula>
     </cfRule>
@@ -5420,12 +5716,12 @@
       <formula>$S$34=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
+  <conditionalFormatting sqref="J10">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>$S9=1</formula>
+      <formula>$S10=1</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>$S8=1</formula>
+      <formula>$S9=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7341,145 +7637,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A49">
-    <cfRule type="expression" dxfId="86" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="19" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B49">
-    <cfRule type="expression" dxfId="84" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="16" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="17" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C49">
-    <cfRule type="expression" dxfId="82" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="12" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:H49">
-    <cfRule type="expression" dxfId="81" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="13" stopIfTrue="1">
       <formula>+#REF!="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D49">
-    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="11" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E49">
-    <cfRule type="expression" dxfId="79" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="10" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F49">
-    <cfRule type="expression" dxfId="78" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G49">
-    <cfRule type="expression" dxfId="77" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H49">
-    <cfRule type="expression" dxfId="76" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I49">
-    <cfRule type="expression" dxfId="75" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="5" stopIfTrue="1">
       <formula>$R3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="14" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J49">
-    <cfRule type="expression" dxfId="73" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="2" stopIfTrue="1">
       <formula>$S3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K49">
-    <cfRule type="expression" dxfId="71" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="3" stopIfTrue="1">
       <formula>$T3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="15" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L49">
-    <cfRule type="expression" dxfId="69" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="1" stopIfTrue="1">
       <formula>$U3="i"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="4" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N6">
-    <cfRule type="expression" dxfId="67" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="31" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O6">
-    <cfRule type="expression" dxfId="66" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="30" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P6">
-    <cfRule type="expression" dxfId="65" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="29" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q6">
-    <cfRule type="expression" dxfId="64" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="28" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R6">
-    <cfRule type="expression" dxfId="63" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="27" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S6">
-    <cfRule type="expression" dxfId="62" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="26" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T6">
-    <cfRule type="expression" dxfId="61" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="25" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U6">
-    <cfRule type="expression" dxfId="60" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V3:V6">
-    <cfRule type="expression" dxfId="59" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="23" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W6">
-    <cfRule type="expression" dxfId="58" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X6">
-    <cfRule type="expression" dxfId="57" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="21" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y6">
-    <cfRule type="expression" dxfId="56" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10988,98 +11284,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A60">
-    <cfRule type="expression" dxfId="55" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="24" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="23">
+    <cfRule type="expression" dxfId="77" priority="23">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="expression" dxfId="53" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="22" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="21">
+    <cfRule type="expression" dxfId="75" priority="21">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C60">
-    <cfRule type="expression" dxfId="51" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="20" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="15">
+    <cfRule type="expression" dxfId="73" priority="15">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D60">
-    <cfRule type="expression" dxfId="49" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="19" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="14">
+    <cfRule type="expression" dxfId="71" priority="14">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E60">
-    <cfRule type="expression" dxfId="47" priority="13">
+    <cfRule type="expression" dxfId="70" priority="13">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="18" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F60">
-    <cfRule type="cellIs" dxfId="45" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F60">
-    <cfRule type="expression" dxfId="43" priority="12">
+    <cfRule type="expression" dxfId="66" priority="12">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="17" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G60">
-    <cfRule type="expression" dxfId="41" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="63" priority="4">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H60">
-    <cfRule type="expression" dxfId="39" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="8" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="3">
+    <cfRule type="expression" dxfId="61" priority="3">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I60">
-    <cfRule type="expression" dxfId="37" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="7" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2">
+    <cfRule type="expression" dxfId="59" priority="2">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J60">
-    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J60">
-    <cfRule type="expression" dxfId="33" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="6" stopIfTrue="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="55" priority="1">
       <formula>$B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>